<commit_message>
Add setup of LIS2DH and logging without persistence to energy consumption
</commit_message>
<xml_diff>
--- a/Energiemessung.xlsx
+++ b/Energiemessung.xlsx
@@ -1,32 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScience\3. Semester\Big Data Anwendungsfaelle\buchwitz\bchwtz-bdcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D83218-1009-49E8-8D56-F7BEFE60863C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E8C83B-5C98-4DC5-BF4A-3480790FB377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{B67F8191-3073-430E-9591-E6550476AFBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B67F8191-3073-430E-9591-E6550476AFBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramm1" sheetId="2" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="17">
   <si>
     <t>Aktion</t>
   </si>
@@ -71,6 +79,12 @@
   </si>
   <si>
     <t>streaming</t>
+  </si>
+  <si>
+    <t>setup</t>
+  </si>
+  <si>
+    <t>without</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1059,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B68182BD-2F11-4830-B599-C602A933FB09}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1056,7 +1070,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305192" cy="6008077"/>
+    <xdr:ext cx="9308171" cy="6017012"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -1382,10 +1396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7993D856-C162-41E2-90DF-FEC8DF5F84B6}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,7 +1489,7 @@
         <v>148</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H19" si="0">E3*F3*G3/1000</f>
+        <f t="shared" ref="H3:H29" si="0">E3*F3*G3/1000</f>
         <v>266.39999999999998</v>
       </c>
     </row>
@@ -1903,6 +1917,276 @@
       <c r="H19" s="1">
         <f t="shared" si="0"/>
         <v>2664</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1">
+        <v>600</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1">
+        <v>29</v>
+      </c>
+      <c r="H20" s="1">
+        <f>E20*F20*G20/1000</f>
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1">
+        <v>600</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1">
+        <v>31</v>
+      </c>
+      <c r="H21" s="1">
+        <f>E21*F21*G21/1000</f>
+        <v>55.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>50</v>
+      </c>
+      <c r="E22" s="1">
+        <v>600</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1">
+        <v>37</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="0"/>
+        <v>66.599999999999994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
+      </c>
+      <c r="E23" s="1">
+        <v>600</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1">
+        <v>48</v>
+      </c>
+      <c r="H23" s="1">
+        <f>E23*F23*G23/1000</f>
+        <v>86.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>200</v>
+      </c>
+      <c r="E24" s="1">
+        <v>600</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1">
+        <v>70</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1">
+        <v>600</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>31</v>
+      </c>
+      <c r="H25" s="1">
+        <f>E25*F25*G25/1000</f>
+        <v>55.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26" s="1">
+        <v>600</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1">
+        <v>35</v>
+      </c>
+      <c r="H26" s="1">
+        <f>E26*F26*G26/1000</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+      <c r="E27" s="1">
+        <v>600</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3</v>
+      </c>
+      <c r="G27" s="1">
+        <v>42</v>
+      </c>
+      <c r="H27" s="1">
+        <f>E27*F27*G27/1000</f>
+        <v>75.599999999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+      <c r="E28" s="1">
+        <v>600</v>
+      </c>
+      <c r="F28" s="1">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1">
+        <v>59</v>
+      </c>
+      <c r="H28" s="1">
+        <f>E28*F28*G28/1000</f>
+        <v>106.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>200</v>
+      </c>
+      <c r="E29" s="1">
+        <v>600</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <v>91</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="0"/>
+        <v>163.80000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>